<commit_message>
Fixed Closed Loop, started stepper control
</commit_message>
<xml_diff>
--- a/Lab3/PlantMath2.xlsx
+++ b/Lab3/PlantMath2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\Documents\MECHA4\MECH423\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306126B0-BFF0-41BC-8EAE-17F991315282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFC12EA-9EA9-4732-BA0D-80D84CD28E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -71,13 +71,67 @@
   <si>
     <t>Tau</t>
   </si>
+  <si>
+    <t>Byte1</t>
+  </si>
+  <si>
+    <t>Byte2</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Hex1</t>
+  </si>
+  <si>
+    <t>Hex2</t>
+  </si>
+  <si>
+    <t>Converted to Int</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>Kenc</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Kp</t>
+  </si>
+  <si>
+    <t>A000</t>
+  </si>
+  <si>
+    <t>Stepper Steps</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.00000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -112,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1890,16 +1944,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1926,16 +1980,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2260,18 +2314,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D818FD15-D729-467A-B703-939A655CDA7C}">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2285,7 +2342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>25</v>
       </c>
@@ -2301,8 +2358,14 @@
         <f>C3/(5*A3/100)</f>
         <v>2.7200000000000005E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>50</v>
       </c>
@@ -2318,8 +2381,15 @@
         <f t="shared" ref="D4:D6" si="0">C4/(5*A4/100)</f>
         <v>3.0400000000000007E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <f>4*2*20/20.4/48</f>
+        <v>0.16339869281045752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>75</v>
       </c>
@@ -2335,8 +2405,15 @@
         <f t="shared" si="0"/>
         <v>3.3523809523809521E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <f>65535/G3</f>
+        <v>532.80487804878044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100</v>
       </c>
@@ -2352,8 +2429,15 @@
         <f t="shared" si="0"/>
         <v>3.428571428571429E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <f>1/B8*1.1</f>
+        <v>46.31578947368422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2367,6 +2451,151 @@
       <c r="D8" s="3">
         <f>AVERAGE(D3:D6)</f>
         <v>3.1352380952380954E-4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9">
+        <f>HEX2DEC(F9)</f>
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>192</v>
+      </c>
+      <c r="D12" t="str">
+        <f>DEC2HEX(B12)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" t="str">
+        <f>DEC2HEX(C12)</f>
+        <v>C0</v>
+      </c>
+      <c r="F12">
+        <f>_xlfn.BITLSHIFT(B12,8)+C12</f>
+        <v>192</v>
+      </c>
+      <c r="G12">
+        <f>F12</f>
+        <v>192</v>
+      </c>
+      <c r="H12">
+        <f>G12/G5</f>
+        <v>0.36035706111238275</v>
+      </c>
+      <c r="I12">
+        <f>F12/G5/(2*20/400)</f>
+        <v>3.6035706111238275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>232</v>
+      </c>
+      <c r="D13" t="str">
+        <f>DEC2HEX(B13)</f>
+        <v>3</v>
+      </c>
+      <c r="E13" t="str">
+        <f>DEC2HEX(C13)</f>
+        <v>E8</v>
+      </c>
+      <c r="F13">
+        <f>_xlfn.BITLSHIFT(B13,8)+C13</f>
+        <v>1000</v>
+      </c>
+      <c r="G13">
+        <f>F13*G4*G5</f>
+        <v>87059.620596205961</v>
+      </c>
+      <c r="H13">
+        <f>G13/G5</f>
+        <v>163.39869281045753</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="e">
+        <f>_xlfn.BITRSHIFT(F14,8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F14">
+        <f>F12/G4/G5</f>
+        <v>2.2053852140077823</v>
+      </c>
+      <c r="G14">
+        <f>G12</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <f>G12-G13</f>
+        <v>-86867.620596205961</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>ABS(G15)*G6</f>
+        <v>4023342.4276137506</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f>_xlfn.BITRSHIFT(65535,8)</f>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Stepper Motor driver to duty cycle and started implementing 2 axis control
</commit_message>
<xml_diff>
--- a/Lab3/PlantMath2.xlsx
+++ b/Lab3/PlantMath2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\Documents\MECHA4\MECH423\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFC12EA-9EA9-4732-BA0D-80D84CD28E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C91391-59B5-4156-9E27-FAC676E220AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -125,13 +125,20 @@
   <si>
     <t>Stepper Steps</t>
   </si>
+  <si>
+    <t>hstomm</t>
+  </si>
+  <si>
+    <t>kdy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -162,11 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2314,10 +2322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D818FD15-D729-467A-B703-939A655CDA7C}">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2499,14 +2507,14 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="C12">
         <v>192</v>
       </c>
       <c r="D12" t="str">
         <f>DEC2HEX(B12)</f>
-        <v>0</v>
+        <v>7E</v>
       </c>
       <c r="E12" t="str">
         <f>DEC2HEX(C12)</f>
@@ -2514,19 +2522,19 @@
       </c>
       <c r="F12">
         <f>_xlfn.BITLSHIFT(B12,8)+C12</f>
-        <v>192</v>
+        <v>32448</v>
       </c>
       <c r="G12">
         <f>F12</f>
-        <v>192</v>
+        <v>32448</v>
       </c>
       <c r="H12">
         <f>G12/G5</f>
-        <v>0.36035706111238275</v>
+        <v>60.90034332799268</v>
       </c>
       <c r="I12">
         <f>F12/G5/(2*20/400)</f>
-        <v>3.6035706111238275</v>
+        <v>609.00343327992675</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2570,11 +2578,11 @@
       </c>
       <c r="F14">
         <f>F12/G4/G5</f>
-        <v>2.2053852140077823</v>
+        <v>372.7101011673152</v>
       </c>
       <c r="G14">
         <f>G12</f>
-        <v>192</v>
+        <v>32448</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2583,19 +2591,52 @@
       </c>
       <c r="G15">
         <f>G12-G13</f>
-        <v>-86867.620596205961</v>
+        <v>-54611.620596205961</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16">
         <f>ABS(G15)*G6</f>
-        <v>4023342.4276137506</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+        <v>2529380.3223505924</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19">
         <f>_xlfn.BITRSHIFT(65535,8)</f>
         <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21">
+        <f>65535/123</f>
+        <v>532.80487804878044</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="4">
+        <f>2*20/400</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>32448</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <f>G23/(G21*G22)</f>
+        <v>609.00343327992675</v>
+      </c>
+      <c r="H24">
+        <f>G21*G22</f>
+        <v>53.280487804878049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed faster clock and tweaking timer interrupts for better performance
</commit_message>
<xml_diff>
--- a/Lab3/PlantMath2.xlsx
+++ b/Lab3/PlantMath2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\Documents\MECHA4\MECH423\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C91391-59B5-4156-9E27-FAC676E220AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D33739-8EF8-4C10-828B-B7D99D28D0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -131,6 +131,15 @@
   <si>
     <t>kdy</t>
   </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
 </sst>
 </file>
 
@@ -138,7 +147,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -174,7 +183,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2322,10 +2331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D818FD15-D729-467A-B703-939A655CDA7C}">
-  <dimension ref="A2:I24"/>
+  <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2507,34 +2516,34 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>126</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>192</v>
+        <v>90</v>
       </c>
       <c r="D12" t="str">
         <f>DEC2HEX(B12)</f>
-        <v>7E</v>
+        <v>2</v>
       </c>
       <c r="E12" t="str">
         <f>DEC2HEX(C12)</f>
-        <v>C0</v>
+        <v>5A</v>
       </c>
       <c r="F12">
         <f>_xlfn.BITLSHIFT(B12,8)+C12</f>
-        <v>32448</v>
+        <v>602</v>
       </c>
       <c r="G12">
         <f>F12</f>
-        <v>32448</v>
+        <v>602</v>
       </c>
       <c r="H12">
         <f>G12/G5</f>
-        <v>60.90034332799268</v>
+        <v>1.1298695353627835</v>
       </c>
       <c r="I12">
         <f>F12/G5/(2*20/400)</f>
-        <v>609.00343327992675</v>
+        <v>11.298695353627833</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2542,30 +2551,30 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>232</v>
+        <v>53</v>
       </c>
       <c r="D13" t="str">
         <f>DEC2HEX(B13)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
         <f>DEC2HEX(C13)</f>
-        <v>E8</v>
+        <v>35</v>
       </c>
       <c r="F13">
         <f>_xlfn.BITLSHIFT(B13,8)+C13</f>
-        <v>1000</v>
+        <v>53</v>
       </c>
       <c r="G13">
         <f>F13*G4*G5</f>
-        <v>87059.620596205961</v>
+        <v>4614.1598915989152</v>
       </c>
       <c r="H13">
         <f>G13/G5</f>
-        <v>163.39869281045753</v>
+        <v>8.6601307189542478</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2578,11 +2587,11 @@
       </c>
       <c r="F14">
         <f>F12/G4/G5</f>
-        <v>372.7101011673152</v>
+        <v>6.9148015564202341</v>
       </c>
       <c r="G14">
         <f>G12</f>
-        <v>32448</v>
+        <v>602</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2591,22 +2600,50 @@
       </c>
       <c r="G15">
         <f>G12-G13</f>
-        <v>-54611.620596205961</v>
+        <v>-4012.1598915989152</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
       <c r="G16">
         <f>ABS(G15)*G6</f>
-        <v>2529380.3223505924</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+        <v>185826.35287405507</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <f>HEX2DEC(B17)</f>
+        <v>189</v>
+      </c>
+      <c r="E17">
+        <f>HEX2DEC(C17)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C19">
         <f>_xlfn.BITRSHIFT(65535,8)</f>
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>29</v>
       </c>
@@ -2615,7 +2652,7 @@
         <v>532.80487804878044</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>28</v>
       </c>
@@ -2624,12 +2661,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G23">
         <v>32448</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G24">
         <f>G23/(G21*G22)</f>
         <v>609.00343327992675</v>
@@ -2637,6 +2674,35 @@
       <c r="H24">
         <f>G21*G22</f>
         <v>53.280487804878049</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>124</v>
+      </c>
+      <c r="C26">
+        <v>162</v>
+      </c>
+      <c r="D26" t="str">
+        <f>DEC2HEX(B26)</f>
+        <v>7C</v>
+      </c>
+      <c r="E26" t="str">
+        <f>DEC2HEX(C26)</f>
+        <v>A2</v>
+      </c>
+      <c r="F26">
+        <f>_xlfn.BITLSHIFT(B26,8)+C26</f>
+        <v>31906</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f>60*G5</f>
+        <v>31968.292682926825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed scaling of steps to work with neg y direction and optimized control loop
</commit_message>
<xml_diff>
--- a/Lab3/PlantMath2.xlsx
+++ b/Lab3/PlantMath2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\Documents\MECHA4\MECH423\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D33739-8EF8-4C10-828B-B7D99D28D0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D2B379-258A-4D96-B43C-AA084B49EC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
   </bookViews>
@@ -2334,7 +2334,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2519,7 +2519,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="D12" t="str">
         <f>DEC2HEX(B12)</f>
@@ -2527,23 +2527,23 @@
       </c>
       <c r="E12" t="str">
         <f>DEC2HEX(C12)</f>
-        <v>5A</v>
+        <v>67</v>
       </c>
       <c r="F12">
         <f>_xlfn.BITLSHIFT(B12,8)+C12</f>
-        <v>602</v>
+        <v>615</v>
       </c>
       <c r="G12">
         <f>F12</f>
-        <v>602</v>
+        <v>615</v>
       </c>
       <c r="H12">
         <f>G12/G5</f>
-        <v>1.1298695353627835</v>
+        <v>1.1542687113756009</v>
       </c>
       <c r="I12">
         <f>F12/G5/(2*20/400)</f>
-        <v>11.298695353627833</v>
+        <v>11.542687113756008</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2551,30 +2551,30 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="D13" t="str">
         <f>DEC2HEX(B13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" t="str">
         <f>DEC2HEX(C13)</f>
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <f>_xlfn.BITLSHIFT(B13,8)+C13</f>
-        <v>53</v>
+        <v>615</v>
       </c>
       <c r="G13">
         <f>F13*G4*G5</f>
-        <v>4614.1598915989152</v>
+        <v>53541.666666666657</v>
       </c>
       <c r="H13">
         <f>G13/G5</f>
-        <v>8.6601307189542478</v>
+        <v>100.49019607843137</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2587,11 +2587,11 @@
       </c>
       <c r="F14">
         <f>F12/G4/G5</f>
-        <v>6.9148015564202341</v>
+        <v>7.064124513618677</v>
       </c>
       <c r="G14">
         <f>G12</f>
-        <v>602</v>
+        <v>615</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="G15">
         <f>G12-G13</f>
-        <v>-4012.1598915989152</v>
+        <v>-52926.666666666657</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2618,10 +2618,10 @@
       </c>
       <c r="G16">
         <f>ABS(G15)*G6</f>
-        <v>185826.35287405507</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2451340.3508771928</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -2637,13 +2637,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C19">
         <f>_xlfn.BITRSHIFT(65535,8)</f>
         <v>255</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <f>H13/H12</f>
+        <v>87.059620596205946</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>29</v>
       </c>
@@ -2652,7 +2656,7 @@
         <v>532.80487804878044</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>28</v>
       </c>
@@ -2661,12 +2665,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G23">
         <v>32448</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G24">
         <f>G23/(G21*G22)</f>
         <v>609.00343327992675</v>
@@ -2676,7 +2680,7 @@
         <v>53.280487804878049</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>31906</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C28">
         <f>60*G5</f>
         <v>31968.292682926825</v>

</xml_diff>

<commit_message>
Final tuning of 2 axis control
</commit_message>
<xml_diff>
--- a/Lab3/PlantMath2.xlsx
+++ b/Lab3/PlantMath2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\Documents\MECHA4\MECH423\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D2B379-258A-4D96-B43C-AA084B49EC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8597C2E0-35C4-4B35-BFFA-A56059323BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
   </bookViews>
@@ -2334,7 +2334,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,34 +2516,34 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="C12">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="D12" t="str">
         <f>DEC2HEX(B12)</f>
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="E12" t="str">
         <f>DEC2HEX(C12)</f>
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <f>_xlfn.BITLSHIFT(B12,8)+C12</f>
-        <v>615</v>
+        <v>37376</v>
       </c>
       <c r="G12">
         <f>F12</f>
-        <v>615</v>
+        <v>37376</v>
       </c>
       <c r="H12">
         <f>G12/G5</f>
-        <v>1.1542687113756009</v>
+        <v>70.149507896543838</v>
       </c>
       <c r="I12">
         <f>F12/G5/(2*20/400)</f>
-        <v>11.542687113756008</v>
+        <v>701.49507896543832</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2551,30 +2551,30 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="D13" t="str">
         <f>DEC2HEX(B13)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
         <f>DEC2HEX(C13)</f>
-        <v>67</v>
+        <v>BA</v>
       </c>
       <c r="F13">
         <f>_xlfn.BITLSHIFT(B13,8)+C13</f>
-        <v>615</v>
+        <v>186</v>
       </c>
       <c r="G13">
         <f>F13*G4*G5</f>
-        <v>53541.666666666657</v>
+        <v>16193.089430894308</v>
       </c>
       <c r="H13">
         <f>G13/G5</f>
-        <v>100.49019607843137</v>
+        <v>30.3921568627451</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2587,11 +2587,11 @@
       </c>
       <c r="F14">
         <f>F12/G4/G5</f>
-        <v>7.064124513618677</v>
+        <v>429.31498832684827</v>
       </c>
       <c r="G14">
         <f>G12</f>
-        <v>615</v>
+        <v>37376</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="G15">
         <f>G12-G13</f>
-        <v>-52926.666666666657</v>
+        <v>21182.91056910569</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="G16">
         <f>ABS(G15)*G6</f>
-        <v>2451340.3508771928</v>
+        <v>981103.22635857947</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -2644,7 +2644,7 @@
       </c>
       <c r="I19">
         <f>H13/H12</f>
-        <v>87.059620596205946</v>
+        <v>0.43324832595500612</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>